<commit_message>
Updated lunch sponsor to 1000
</commit_message>
<xml_diff>
--- a/SponsorshipInformation.xlsx
+++ b/SponsorshipInformation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brao\Documents\Conference\JSConference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\jsfriendsconf\ConferenceDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEB00E0-B2EF-4F12-9B75-01A4FD27E9F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A2B046-7E1F-46C9-8AF6-B22EC617F7DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{69EEFE14-B81E-4240-9D04-B478FAF380F5}"/>
   </bookViews>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81520146-8CE7-407C-808E-551874B77442}">
   <dimension ref="B3:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="7">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Updated descriptions of sponsorship levels
</commit_message>
<xml_diff>
--- a/SponsorshipInformation.xlsx
+++ b/SponsorshipInformation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\jsfriendsconf\ConferenceDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\JSFriendsConf\ConferenceDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A2B046-7E1F-46C9-8AF6-B22EC617F7DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE12EFE-24CD-4740-83D7-9048729F2B53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{69EEFE14-B81E-4240-9D04-B478FAF380F5}"/>
   </bookViews>
@@ -58,10 +58,6 @@
     <t>Bronze Sponsor</t>
   </si>
   <si>
-    <t>1. Display of your organization logo in our  website Sponsors page. You can provide us with image and link.
-2. Mention in 1 social media posts (Twitter, LinkedIn)</t>
-  </si>
-  <si>
     <t>Speaker Travel Sponsor</t>
   </si>
   <si>
@@ -71,39 +67,42 @@
     <t>Sponsorship Information</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Verbal acknowledgment of your sponsorship at the event during lunch.
-2. Display of your organization logo in our website Additional Sponsors section. You can provide us with image and link.
-3. Display of your organization logo in presentation deck in Lunch Room.
+    <t>Speaker Dinner Sponsor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Mention of your organization in emails to event attendees
+2. Branded swag materials you provide included in attendee kit
+3. Verbal acknowledgment of your sponsorship at the event during Lunch
+4.  Display of your organization logo in our website Sponsors page
+5. Mention in at least 5 social media posts
+6. Preferred location for your booth at the conference
+8. Display of your logo in Eventbrite ticketing page
 </t>
   </si>
   <si>
-    <t>Speaker Dinner Sponsor</t>
-  </si>
-  <si>
-    <t>1. Verbal acknowledgment of your sponsorship during Speaker Dinner.
-2. Display of your organization logo in our website Additional Sponsors section. You can provide us with image and link.
-3. Display of your organization logo in presentation deck in Lunch Room.</t>
-  </si>
-  <si>
-    <t>1.  Display of your organization logo in our website Additional Sponsors Section. You can provide us with image and link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Mention of your organization in emails to event attendees
-2. Provide your branded Swag Materials to Participants in attendee kit.
-3. Verbal acknowledgment of your sponsorship at the event during Lunch and during workshop
-4.  Display of your organization logo in our website Sponsors page. You can provide us with image and your website link.
-5. Mention in 5 social media posts for 2 months until Conference (Twitter, LinkedIn)
-6. Set up your Organization Booth, Max -3 booth staff at your preferred location
-7. Display of Organization Logo in Session Rooms
-8. Display of your logo in Event brite ticketing page
+    <t>1. Mention of your organization in emails to event attendees 
+2. Verbal acknowledgment of your sponsorship at the event during Lunch
+3. Display of your organization logo in our website Sponsors page
+4. Mention in at least 2 social media posts
+5. Space for your organization's booth at the conference</t>
+  </si>
+  <si>
+    <t>1. Display of your organization logo in our  website Sponsors page
+2. Mention in at least 1 social media post</t>
+  </si>
+  <si>
+    <t>1.  Display of your organization logo in our website Additional Sponsors Section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Verbal acknowledgment of your sponsorship at the event during lunch
+2. Display of your organization logo in our website Sponsors page
+3. Display of your organization logo in presentation deck at lunch
 </t>
   </si>
   <si>
-    <t>1. Mention of your organization in emails to event attendees 
-2. Verbal acknowledgment of your sponsorship at the event during Lunch.
-3. Display of your organization logo in our website Sponsors page. You can provide us with image and link.
-4. Mention in 2 social media posts for 2 months until Conference (Twitter, LinkedIn)
-5. Set up your Organization Booth, Max-2 booth staff at assigned location</t>
+    <t>1. Verbal acknowledgment of your sponsorship during Speaker Dinner
+2. Display of your organization logo in our website Sponsors section
+3. Display of your organization logo in presentation deck in Lunch Room</t>
   </si>
 </sst>
 </file>
@@ -533,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81520146-8CE7-407C-808E-551874B77442}">
   <dimension ref="B3:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +547,7 @@
   <sheetData>
     <row r="3" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -579,7 +578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
@@ -590,7 +589,7 @@
         <v>2500</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -605,11 +604,11 @@
         <v>1500</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
@@ -620,13 +619,13 @@
         <v>500</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="6">
         <v>22</v>
@@ -641,7 +640,7 @@
     </row>
     <row r="10" spans="2:6" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="6">
         <v>3</v>
@@ -650,13 +649,13 @@
         <v>1000</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -665,7 +664,7 @@
         <v>600</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2"/>
     </row>

</xml_diff>